<commit_message>
add auto calculate, select2, modify database siswa pembayaran
</commit_message>
<xml_diff>
--- a/upload/format_siswa.xlsx
+++ b/upload/format_siswa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="815">
   <si>
     <t>no</t>
   </si>
@@ -2451,6 +2451,24 @@
   </si>
   <si>
     <t>IPS</t>
+  </si>
+  <si>
+    <t>status keuangan</t>
+  </si>
+  <si>
+    <t>Lunas</t>
+  </si>
+  <si>
+    <t>2002-10-12</t>
+  </si>
+  <si>
+    <t>9348573</t>
+  </si>
+  <si>
+    <t>User Coba</t>
+  </si>
+  <si>
+    <t>Belum Lunas</t>
   </si>
 </sst>
 </file>
@@ -2528,7 +2546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2541,6 +2559,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2855,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G279"/>
+  <dimension ref="A1:H280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="E279" sqref="E279"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A280" sqref="A280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,7 +2890,7 @@
     <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2891,8 +2912,11 @@
       <c r="G1" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2914,8 +2938,11 @@
       <c r="G2" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2937,8 +2964,11 @@
       <c r="G3" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2960,8 +2990,11 @@
       <c r="G4" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2983,8 +3016,11 @@
       <c r="G5" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3006,8 +3042,11 @@
       <c r="G6" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3029,8 +3068,11 @@
       <c r="G7" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3052,8 +3094,11 @@
       <c r="G8" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3075,8 +3120,11 @@
       <c r="G9" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3098,8 +3146,11 @@
       <c r="G10" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3121,8 +3172,11 @@
       <c r="G11" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3144,8 +3198,11 @@
       <c r="G12" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3167,8 +3224,11 @@
       <c r="G13" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3190,8 +3250,11 @@
       <c r="G14" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3213,8 +3276,11 @@
       <c r="G15" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3236,8 +3302,11 @@
       <c r="G16" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3259,8 +3328,11 @@
       <c r="G17" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3282,8 +3354,11 @@
       <c r="G18" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3305,8 +3380,11 @@
       <c r="G19" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3328,8 +3406,11 @@
       <c r="G20" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3351,8 +3432,11 @@
       <c r="G21" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3374,8 +3458,11 @@
       <c r="G22" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3397,8 +3484,11 @@
       <c r="G23" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3420,8 +3510,11 @@
       <c r="G24" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3443,8 +3536,11 @@
       <c r="G25" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3466,8 +3562,11 @@
       <c r="G26" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3489,8 +3588,11 @@
       <c r="G27" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3512,8 +3614,11 @@
       <c r="G28" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3535,8 +3640,11 @@
       <c r="G29" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3558,8 +3666,11 @@
       <c r="G30" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3581,8 +3692,11 @@
       <c r="G31" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3604,8 +3718,11 @@
       <c r="G32" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3627,8 +3744,11 @@
       <c r="G33" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3650,8 +3770,11 @@
       <c r="G34" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3673,8 +3796,11 @@
       <c r="G35" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3696,8 +3822,11 @@
       <c r="G36" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3719,8 +3848,11 @@
       <c r="G37" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3742,8 +3874,11 @@
       <c r="G38" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3765,8 +3900,11 @@
       <c r="G39" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3788,8 +3926,11 @@
       <c r="G40" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3811,8 +3952,11 @@
       <c r="G41" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3834,8 +3978,11 @@
       <c r="G42" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3857,8 +4004,11 @@
       <c r="G43" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3880,8 +4030,11 @@
       <c r="G44" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3903,8 +4056,11 @@
       <c r="G45" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3926,8 +4082,11 @@
       <c r="G46" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3949,8 +4108,11 @@
       <c r="G47" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3972,8 +4134,11 @@
       <c r="G48" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3995,8 +4160,11 @@
       <c r="G49" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4018,8 +4186,11 @@
       <c r="G50" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4041,8 +4212,11 @@
       <c r="G51" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4064,8 +4238,11 @@
       <c r="G52" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4087,8 +4264,11 @@
       <c r="G53" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4110,8 +4290,11 @@
       <c r="G54" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4133,8 +4316,11 @@
       <c r="G55" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4156,8 +4342,11 @@
       <c r="G56" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4179,8 +4368,11 @@
       <c r="G57" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4202,8 +4394,11 @@
       <c r="G58" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4225,8 +4420,11 @@
       <c r="G59" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4248,8 +4446,11 @@
       <c r="G60" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4271,8 +4472,11 @@
       <c r="G61" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4294,8 +4498,11 @@
       <c r="G62" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4317,8 +4524,11 @@
       <c r="G63" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4340,8 +4550,11 @@
       <c r="G64" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4363,8 +4576,11 @@
       <c r="G65" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4386,8 +4602,11 @@
       <c r="G66" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4409,8 +4628,11 @@
       <c r="G67" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4432,8 +4654,11 @@
       <c r="G68" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4455,8 +4680,11 @@
       <c r="G69" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4478,8 +4706,11 @@
       <c r="G70" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4501,8 +4732,11 @@
       <c r="G71" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4524,8 +4758,11 @@
       <c r="G72" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4547,8 +4784,11 @@
       <c r="G73" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4570,8 +4810,11 @@
       <c r="G74" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4593,8 +4836,11 @@
       <c r="G75" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4616,8 +4862,11 @@
       <c r="G76" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4639,8 +4888,11 @@
       <c r="G77" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4662,8 +4914,11 @@
       <c r="G78" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4685,8 +4940,11 @@
       <c r="G79" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4708,8 +4966,11 @@
       <c r="G80" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4731,8 +4992,11 @@
       <c r="G81" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4754,8 +5018,11 @@
       <c r="G82" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4777,8 +5044,11 @@
       <c r="G83" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4800,8 +5070,11 @@
       <c r="G84" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4823,8 +5096,11 @@
       <c r="G85" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4846,8 +5122,11 @@
       <c r="G86" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4869,8 +5148,11 @@
       <c r="G87" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4892,8 +5174,11 @@
       <c r="G88" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4915,8 +5200,11 @@
       <c r="G89" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4938,8 +5226,11 @@
       <c r="G90" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4961,8 +5252,11 @@
       <c r="G91" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4984,8 +5278,11 @@
       <c r="G92" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5007,8 +5304,11 @@
       <c r="G93" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5030,8 +5330,11 @@
       <c r="G94" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5053,8 +5356,11 @@
       <c r="G95" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5076,8 +5382,11 @@
       <c r="G96" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5099,8 +5408,11 @@
       <c r="G97" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5122,8 +5434,11 @@
       <c r="G98" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5145,8 +5460,11 @@
       <c r="G99" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5168,8 +5486,11 @@
       <c r="G100" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5191,8 +5512,11 @@
       <c r="G101" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5214,8 +5538,11 @@
       <c r="G102" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5237,8 +5564,11 @@
       <c r="G103" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5260,8 +5590,11 @@
       <c r="G104" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5283,8 +5616,11 @@
       <c r="G105" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5306,8 +5642,11 @@
       <c r="G106" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5329,8 +5668,11 @@
       <c r="G107" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5352,8 +5694,11 @@
       <c r="G108" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5375,8 +5720,11 @@
       <c r="G109" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5398,8 +5746,11 @@
       <c r="G110" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5421,8 +5772,11 @@
       <c r="G111" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5444,8 +5798,11 @@
       <c r="G112" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5467,8 +5824,11 @@
       <c r="G113" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5490,8 +5850,11 @@
       <c r="G114" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5513,8 +5876,11 @@
       <c r="G115" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5536,8 +5902,11 @@
       <c r="G116" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5559,8 +5928,11 @@
       <c r="G117" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5582,8 +5954,11 @@
       <c r="G118" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5605,8 +5980,11 @@
       <c r="G119" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5628,8 +6006,11 @@
       <c r="G120" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5651,8 +6032,11 @@
       <c r="G121" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5674,8 +6058,11 @@
       <c r="G122" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5697,8 +6084,11 @@
       <c r="G123" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5720,8 +6110,11 @@
       <c r="G124" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5743,8 +6136,11 @@
       <c r="G125" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5766,8 +6162,11 @@
       <c r="G126" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5789,8 +6188,11 @@
       <c r="G127" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5812,8 +6214,11 @@
       <c r="G128" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5835,8 +6240,11 @@
       <c r="G129" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5858,8 +6266,11 @@
       <c r="G130" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5881,8 +6292,11 @@
       <c r="G131" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5904,8 +6318,11 @@
       <c r="G132" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5927,8 +6344,11 @@
       <c r="G133" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5950,8 +6370,11 @@
       <c r="G134" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5973,8 +6396,11 @@
       <c r="G135" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5996,8 +6422,11 @@
       <c r="G136" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -6019,8 +6448,11 @@
       <c r="G137" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -6042,8 +6474,11 @@
       <c r="G138" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -6065,8 +6500,11 @@
       <c r="G139" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -6088,8 +6526,11 @@
       <c r="G140" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -6111,8 +6552,11 @@
       <c r="G141" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -6134,8 +6578,11 @@
       <c r="G142" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -6157,8 +6604,11 @@
       <c r="G143" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -6180,8 +6630,11 @@
       <c r="G144" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6203,8 +6656,11 @@
       <c r="G145" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6226,8 +6682,11 @@
       <c r="G146" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6249,8 +6708,11 @@
       <c r="G147" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6272,8 +6734,11 @@
       <c r="G148" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6295,8 +6760,11 @@
       <c r="G149" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6318,8 +6786,11 @@
       <c r="G150" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6341,8 +6812,11 @@
       <c r="G151" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6364,8 +6838,11 @@
       <c r="G152" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6387,8 +6864,11 @@
       <c r="G153" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6410,8 +6890,11 @@
       <c r="G154" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6433,8 +6916,11 @@
       <c r="G155" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H155" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6456,8 +6942,11 @@
       <c r="G156" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H156" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6479,8 +6968,11 @@
       <c r="G157" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H157" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6502,8 +6994,11 @@
       <c r="G158" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H158" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6525,8 +7020,11 @@
       <c r="G159" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H159" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6548,8 +7046,11 @@
       <c r="G160" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H160" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6571,8 +7072,11 @@
       <c r="G161" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H161" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6594,8 +7098,11 @@
       <c r="G162" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H162" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6617,8 +7124,11 @@
       <c r="G163" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H163" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6640,8 +7150,11 @@
       <c r="G164" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6663,8 +7176,11 @@
       <c r="G165" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H165" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6686,8 +7202,11 @@
       <c r="G166" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H166" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6709,8 +7228,11 @@
       <c r="G167" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H167" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6732,8 +7254,11 @@
       <c r="G168" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H168" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6755,8 +7280,11 @@
       <c r="G169" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H169" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6778,8 +7306,11 @@
       <c r="G170" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H170" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6801,8 +7332,11 @@
       <c r="G171" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H171" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6824,8 +7358,11 @@
       <c r="G172" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H172" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6847,8 +7384,11 @@
       <c r="G173" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H173" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6870,8 +7410,11 @@
       <c r="G174" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H174" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6893,8 +7436,11 @@
       <c r="G175" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H175" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6916,8 +7462,11 @@
       <c r="G176" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H176" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6939,8 +7488,11 @@
       <c r="G177" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H177" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6962,8 +7514,11 @@
       <c r="G178" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H178" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6985,8 +7540,11 @@
       <c r="G179" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H179" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -7008,8 +7566,11 @@
       <c r="G180" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H180" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7031,8 +7592,11 @@
       <c r="G181" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H181" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7054,8 +7618,11 @@
       <c r="G182" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H182" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -7077,8 +7644,11 @@
       <c r="G183" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H183" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7100,8 +7670,11 @@
       <c r="G184" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H184" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7123,8 +7696,11 @@
       <c r="G185" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H185" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -7146,8 +7722,11 @@
       <c r="G186" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H186" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -7169,8 +7748,11 @@
       <c r="G187" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H187" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7192,8 +7774,11 @@
       <c r="G188" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7215,8 +7800,11 @@
       <c r="G189" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H189" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -7238,8 +7826,11 @@
       <c r="G190" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H190" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -7261,8 +7852,11 @@
       <c r="G191" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H191" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -7284,8 +7878,11 @@
       <c r="G192" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H192" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -7307,8 +7904,11 @@
       <c r="G193" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H193" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -7330,8 +7930,11 @@
       <c r="G194" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H194" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -7353,8 +7956,11 @@
       <c r="G195" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H195" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -7376,8 +7982,11 @@
       <c r="G196" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H196" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -7399,8 +8008,11 @@
       <c r="G197" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H197" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -7422,8 +8034,11 @@
       <c r="G198" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H198" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -7445,8 +8060,11 @@
       <c r="G199" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H199" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -7468,8 +8086,11 @@
       <c r="G200" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H200" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7491,8 +8112,11 @@
       <c r="G201" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H201" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -7514,8 +8138,11 @@
       <c r="G202" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H202" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -7537,8 +8164,11 @@
       <c r="G203" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H203" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -7560,8 +8190,11 @@
       <c r="G204" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H204" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -7583,8 +8216,11 @@
       <c r="G205" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H205" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -7606,8 +8242,11 @@
       <c r="G206" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H206" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -7629,8 +8268,11 @@
       <c r="G207" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H207" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -7652,8 +8294,11 @@
       <c r="G208" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H208" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -7675,8 +8320,11 @@
       <c r="G209" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H209" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7698,8 +8346,11 @@
       <c r="G210" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H210" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7721,8 +8372,11 @@
       <c r="G211" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H211" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7744,8 +8398,11 @@
       <c r="G212" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H212" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7767,8 +8424,11 @@
       <c r="G213" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H213" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7790,8 +8450,11 @@
       <c r="G214" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H214" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -7813,8 +8476,11 @@
       <c r="G215" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H215" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -7836,8 +8502,11 @@
       <c r="G216" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H216" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -7859,8 +8528,11 @@
       <c r="G217" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H217" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -7882,8 +8554,11 @@
       <c r="G218" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H218" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -7905,8 +8580,11 @@
       <c r="G219" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H219" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -7928,8 +8606,11 @@
       <c r="G220" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H220" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -7951,8 +8632,11 @@
       <c r="G221" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H221" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -7974,8 +8658,11 @@
       <c r="G222" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H222" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -7997,8 +8684,11 @@
       <c r="G223" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H223" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -8020,8 +8710,11 @@
       <c r="G224" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H224" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -8043,8 +8736,11 @@
       <c r="G225" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H225" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -8066,8 +8762,11 @@
       <c r="G226" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H226" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -8089,8 +8788,11 @@
       <c r="G227" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H227" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -8112,8 +8814,11 @@
       <c r="G228" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H228" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -8135,8 +8840,11 @@
       <c r="G229" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H229" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -8158,8 +8866,11 @@
       <c r="G230" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H230" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -8181,8 +8892,11 @@
       <c r="G231" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H231" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -8204,8 +8918,11 @@
       <c r="G232" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H232" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -8227,8 +8944,11 @@
       <c r="G233" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H233" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -8250,8 +8970,11 @@
       <c r="G234" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H234" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -8273,8 +8996,11 @@
       <c r="G235" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H235" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -8296,8 +9022,11 @@
       <c r="G236" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H236" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -8319,8 +9048,11 @@
       <c r="G237" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H237" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -8342,8 +9074,11 @@
       <c r="G238" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H238" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -8365,8 +9100,11 @@
       <c r="G239" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H239" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
@@ -8388,8 +9126,11 @@
       <c r="G240" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H240" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -8411,8 +9152,11 @@
       <c r="G241" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H241" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
@@ -8434,8 +9178,11 @@
       <c r="G242" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H242" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -8457,8 +9204,11 @@
       <c r="G243" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H243" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -8480,8 +9230,11 @@
       <c r="G244" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H244" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -8503,8 +9256,11 @@
       <c r="G245" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H245" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -8526,8 +9282,11 @@
       <c r="G246" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H246" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -8549,8 +9308,11 @@
       <c r="G247" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H247" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -8572,8 +9334,11 @@
       <c r="G248" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H248" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -8595,8 +9360,11 @@
       <c r="G249" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H249" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -8618,8 +9386,11 @@
       <c r="G250" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H250" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -8641,8 +9412,11 @@
       <c r="G251" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H251" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -8664,8 +9438,11 @@
       <c r="G252" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H252" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -8687,8 +9464,11 @@
       <c r="G253" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H253" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -8710,8 +9490,11 @@
       <c r="G254" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H254" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -8733,8 +9516,11 @@
       <c r="G255" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H255" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -8756,8 +9542,11 @@
       <c r="G256" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
@@ -8779,8 +9568,11 @@
       <c r="G257" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H257" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
@@ -8802,8 +9594,11 @@
       <c r="G258" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H258" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
@@ -8825,8 +9620,11 @@
       <c r="G259" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H259" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
@@ -8848,8 +9646,11 @@
       <c r="G260" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H260" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
@@ -8871,8 +9672,11 @@
       <c r="G261" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="262" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H261" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
@@ -8894,8 +9698,11 @@
       <c r="G262" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="263" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H262" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
@@ -8917,8 +9724,11 @@
       <c r="G263" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="264" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H263" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>263</v>
       </c>
@@ -8940,8 +9750,11 @@
       <c r="G264" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="265" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H264" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
@@ -8963,8 +9776,11 @@
       <c r="G265" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="266" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H265" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
@@ -8986,8 +9802,11 @@
       <c r="G266" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="267" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H266" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
@@ -9009,8 +9828,11 @@
       <c r="G267" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="268" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H267" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
@@ -9032,8 +9854,11 @@
       <c r="G268" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="269" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H268" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
@@ -9055,8 +9880,11 @@
       <c r="G269" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="270" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H269" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
@@ -9078,8 +9906,11 @@
       <c r="G270" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="271" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H270" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
@@ -9101,8 +9932,11 @@
       <c r="G271" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="272" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H271" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
@@ -9124,8 +9958,11 @@
       <c r="G272" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="273" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H272" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
@@ -9147,8 +9984,11 @@
       <c r="G273" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="274" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H273" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
@@ -9170,8 +10010,11 @@
       <c r="G274" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="275" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H274" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
@@ -9193,8 +10036,11 @@
       <c r="G275" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="276" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H275" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
@@ -9216,8 +10062,11 @@
       <c r="G276" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="277" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H276" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
@@ -9239,8 +10088,11 @@
       <c r="G277" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="278" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H277" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -9262,8 +10114,11 @@
       <c r="G278" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="279" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H278" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -9284,6 +10139,35 @@
       </c>
       <c r="G279" t="s">
         <v>808</v>
+      </c>
+      <c r="H279" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" s="2">
+        <v>789456</v>
+      </c>
+      <c r="C280" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="D280" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="E280" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="F280" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="G280" t="s">
+        <v>808</v>
+      </c>
+      <c r="H280" t="s">
+        <v>814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>